<commit_message>
Adding sampleData on file upload + error messages
</commit_message>
<xml_diff>
--- a/public/invoice-template.xlsx
+++ b/public/invoice-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B11B8-7E4B-4FFA-8AD2-4533F007DA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0C693E-BB14-43D1-9A54-AB5EDB511DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,15 +116,9 @@
     <t>{paymentTerms}</t>
   </si>
   <si>
-    <t>{qty}</t>
-  </si>
-  <si>
     <t>{description}</t>
   </si>
   <si>
-    <t>{price}</t>
-  </si>
-  <si>
     <t>{#sales}{/sales}</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>{website}</t>
   </si>
   <si>
-    <t>{taxRatePercent}</t>
-  </si>
-  <si>
     <t>{clientPostCode} {clientCity}</t>
   </si>
   <si>
@@ -159,6 +150,15 @@
   </si>
   <si>
     <t>{email}</t>
+  </si>
+  <si>
+    <t>{=qty}</t>
+  </si>
+  <si>
+    <t>{=price}</t>
+  </si>
+  <si>
+    <t>{=taxRatePercent}</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode=";;;"/>
     <numFmt numFmtId="167" formatCode="_(&quot;€&quot;* #,##0.00_);_(&quot;€&quot;* \(#,##0.00\);_(&quot;€&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -654,6 +654,9 @@
     <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,9 +673,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -683,42 +683,6 @@
     <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1" tint="0.14999847407452621"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -744,7 +708,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color theme="5"/>
@@ -860,6 +824,42 @@
         <family val="2"/>
         <scheme val="major"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1159,7 +1159,7 @@
     <tableColumn id="1" xr3:uid="{3EE7F6C8-5045-4864-B814-17FE69D6126B}" name="Salesperson" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{4C8D115E-5E41-4579-9149-DD7283E86948}" name="Job" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{B06CD4EE-D904-4883-BEEC-560EEC12BE98}" name="Payment Terms" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{D0E2D0D1-7103-4735-ACBD-A8E1FAD28416}" name="Due Date" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{D0E2D0D1-7103-4735-ACBD-A8E1FAD28416}" name="Due Date" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1171,7 +1171,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8196D5F1-2ABD-4EF6-A88E-F87162538248}" name="InvoiceDetails" displayName="InvoiceDetails" ref="B15:E19" totalsRowCount="1" headerRowDxfId="6" headerRowBorderDxfId="5" headerRowCellStyle="Normal 5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8196D5F1-2ABD-4EF6-A88E-F87162538248}" name="InvoiceDetails" displayName="InvoiceDetails" ref="B15:E19" totalsRowCount="1" headerRowDxfId="5" headerRowBorderDxfId="4" headerRowCellStyle="Normal 5">
   <autoFilter ref="B15:E18" xr:uid="{79A78173-9F3F-4C5F-95F6-0CE1DD164C02}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1180,9 +1180,9 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CEF46200-F3EF-4D1F-B00D-A6B60C836CF9}" name="Qty"/>
-    <tableColumn id="2" xr3:uid="{69D9074F-70ED-4717-BB8F-D8C3286A77A9}" name="Description" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{749DD0E1-EA89-44CC-A16E-6C6D83A4C1A0}" name="Unit Price" totalsRowLabel="Total" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{8CCE9C0A-57CA-47AA-BAAD-ED99DC6594A8}" name="Line Total" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="2" xr3:uid="{69D9074F-70ED-4717-BB8F-D8C3286A77A9}" name="Description" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{749DD0E1-EA89-44CC-A16E-6C6D83A4C1A0}" name="Unit Price" totalsRowLabel="Total" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8CCE9C0A-57CA-47AA-BAAD-ED99DC6594A8}" name="Line Total" totalsRowFunction="custom" totalsRowDxfId="0">
       <totalsRowFormula>IF(SUM(E17)&gt;0,SUM((E17*E18)+E17),"")</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1508,21 +1508,21 @@
     </row>
     <row r="2" spans="1:7" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="53" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="1:7" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1546,7 @@
     <row r="5" spans="1:7" s="3" customFormat="1" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="27" t="s">
@@ -1562,7 +1562,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1571,7 +1571,7 @@
       <c r="A7" s="30"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1580,7 +1580,7 @@
       <c r="A8" s="30"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1589,7 +1589,7 @@
       <c r="A9" s="30"/>
       <c r="B9" s="4"/>
       <c r="C9" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1598,7 +1598,7 @@
       <c r="A10" s="30"/>
       <c r="B10" s="4"/>
       <c r="C10" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1635,12 +1635,12 @@
       <c r="D13" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="52" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1668,20 +1668,20 @@
     <row r="16" spans="1:7" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
       <c r="B16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>29</v>
-      </c>
       <c r="D16" s="48" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E16" s="49" t="str">
         <f t="shared" ref="E16" si="0">IF(SUM(B16)&gt;0,SUM(B16*D16),"")</f>
         <v/>
       </c>
       <c r="G16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1718,10 +1718,10 @@
     </row>
     <row r="20" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="33"/>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="56"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="40" t="str">
         <f>B3</f>
         <v>{companyName}</v>
@@ -1737,28 +1737,28 @@
     </row>
     <row r="22" spans="1:5" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35"/>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
       <c r="C23" s="46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="11"/>
@@ -1808,35 +1808,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2124,27 +2095,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A96BE63F-19C3-420D-9D87-FB3F93D941D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEA82F4-01CD-462F-8B19-F2702D004A2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B520A4B0-A8DD-427B-A39A-42A82F52AF6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2163,4 +2143,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEA82F4-01CD-462F-8B19-F2702D004A2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A96BE63F-19C3-420D-9D87-FB3F93D941D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>